<commit_message>
added code for deleting product and goods
</commit_message>
<xml_diff>
--- a/Data/data.xlsx
+++ b/Data/data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>13.6</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -473,7 +473,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -488,7 +488,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2.75</v>
+        <v>2.65</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -503,7 +503,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>4.7</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -553,6 +553,21 @@
       <c r="C8" t="inlineStr">
         <is>
           <t>piece</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>sugar</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>kg</t>
         </is>
       </c>
     </row>
@@ -567,7 +582,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -615,7 +630,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">
@@ -680,7 +695,20 @@
         <v>0.6</v>
       </c>
       <c r="C8" t="n">
-        <v>10</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>oreo</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added change product name
</commit_message>
<xml_diff>
--- a/Data/data.xlsx
+++ b/Data/data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -566,6 +566,21 @@
         <v>2</v>
       </c>
       <c r="C9" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>salt</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="inlineStr">
         <is>
           <t>kg</t>
         </is>
@@ -582,7 +597,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -711,6 +726,19 @@
         <v>0</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>croissant</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>